<commit_message>
New dependancies like window based automation and Image automation are added with few code changes
</commit_message>
<xml_diff>
--- a/target/test-classes/com/v3mobi/testData/Login.xlsx
+++ b/target/test-classes/com/v3mobi/testData/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="15120" windowHeight="8076" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="15120" windowHeight="8076"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:O26"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
   <si>
     <t>TC001</t>
   </si>
@@ -28,9 +27,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>manager</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -56,18 +52,6 @@
   </si>
   <si>
     <t>runMode</t>
-  </si>
-  <si>
-    <t>mdcager</t>
-  </si>
-  <si>
-    <t>manadsger</t>
-  </si>
-  <si>
-    <t>manadsdger</t>
-  </si>
-  <si>
-    <t>manasddsdger</t>
   </si>
   <si>
     <t>Vikas</t>
@@ -412,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -425,16 +409,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -445,10 +429,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -459,52 +443,52 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -516,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -528,16 +512,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -545,13 +529,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -562,52 +546,52 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>